<commit_message>
Corrected bug in budgetController and generateStatementController
</commit_message>
<xml_diff>
--- a/Backend/src/api/controllers/statement_1.xlsx
+++ b/Backend/src/api/controllers/statement_1.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -34,19 +34,22 @@
     <t>2024-06-02</t>
   </si>
   <si>
+    <t>Expense</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Panda Express</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>2024-05-30</t>
+  </si>
+  <si>
     <t>Income</t>
-  </si>
-  <si>
-    <t>Food</t>
-  </si>
-  <si>
-    <t>Panda Express</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>2024-05-30</t>
   </si>
   <si>
     <t>Essays</t>
@@ -521,16 +524,16 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -538,7 +541,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -550,7 +553,7 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
@@ -558,7 +561,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -567,10 +570,10 @@
         <v>60</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>

</xml_diff>